<commit_message>
Fixed TemplateParser Bug and made GUI Manager show missing fields without json object
</commit_message>
<xml_diff>
--- a/testFiles/ParseTestFiles/client_profileMissing.xlsx
+++ b/testFiles/ParseTestFiles/client_profileMissing.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="51">
   <si>
     <t>Yes</t>
   </si>
@@ -164,6 +164,12 @@
 iCARE - Immigration Contribution Agreement Reporting Environment
 Client Profile
 </t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>d</t>
   </si>
 </sst>
 </file>
@@ -589,8 +595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q2503"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15"/>
@@ -614,7 +620,7 @@
     <col min="18" max="16384" width="8.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="8" customFormat="1" ht="99.95" customHeight="1">
+    <row r="1" spans="1:17" s="8" customFormat="1" ht="99.75" customHeight="1">
       <c r="A1" s="9" t="s">
         <v>48</v>
       </c>
@@ -806,7 +812,9 @@
       <c r="M5" s="3"/>
       <c r="N5" s="2"/>
       <c r="O5" s="3"/>
-      <c r="P5" s="2"/>
+      <c r="P5" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="Q5" s="2"/>
     </row>
     <row r="6" spans="1:17">
@@ -850,7 +858,9 @@
     <row r="8" spans="1:17">
       <c r="A8" s="3"/>
       <c r="B8" s="2"/>
-      <c r="C8" s="3"/>
+      <c r="C8" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="2"/>
@@ -888,8 +898,12 @@
     <row r="10" spans="1:17">
       <c r="A10" s="3"/>
       <c r="B10" s="2"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
+      <c r="C10" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="E10" s="3"/>
       <c r="F10" s="2"/>
       <c r="G10" s="3"/>
@@ -908,7 +922,9 @@
       <c r="A11" s="3"/>
       <c r="B11" s="2"/>
       <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
+      <c r="D11" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="E11" s="3"/>
       <c r="F11" s="2"/>
       <c r="G11" s="3"/>
@@ -926,7 +942,9 @@
     <row r="12" spans="1:17">
       <c r="A12" s="3"/>
       <c r="B12" s="2"/>
-      <c r="C12" s="3"/>
+      <c r="C12" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="2"/>
@@ -945,7 +963,9 @@
     <row r="13" spans="1:17">
       <c r="A13" s="3"/>
       <c r="B13" s="2"/>
-      <c r="C13" s="3"/>
+      <c r="C13" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="2"/>
@@ -965,7 +985,9 @@
       <c r="A14" s="3"/>
       <c r="B14" s="2"/>
       <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
+      <c r="D14" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="E14" s="3"/>
       <c r="F14" s="2"/>
       <c r="G14" s="3"/>
@@ -984,7 +1006,9 @@
       <c r="A15" s="3"/>
       <c r="B15" s="2"/>
       <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
+      <c r="D15" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="E15" s="3"/>
       <c r="F15" s="2"/>
       <c r="G15" s="3"/>
@@ -1002,7 +1026,9 @@
     <row r="16" spans="1:17">
       <c r="A16" s="3"/>
       <c r="B16" s="2"/>
-      <c r="C16" s="3"/>
+      <c r="C16" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="2"/>
@@ -1021,7 +1047,9 @@
     <row r="17" spans="1:17">
       <c r="A17" s="3"/>
       <c r="B17" s="2"/>
-      <c r="C17" s="3"/>
+      <c r="C17" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="2"/>
@@ -1040,7 +1068,9 @@
     <row r="18" spans="1:17">
       <c r="A18" s="3"/>
       <c r="B18" s="2"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="2"/>
@@ -1059,7 +1089,9 @@
     <row r="19" spans="1:17">
       <c r="A19" s="3"/>
       <c r="B19" s="2"/>
-      <c r="C19" s="3"/>
+      <c r="C19" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="2"/>
@@ -1079,7 +1111,9 @@
       <c r="A20" s="3"/>
       <c r="B20" s="2"/>
       <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
+      <c r="D20" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="E20" s="3"/>
       <c r="F20" s="2"/>
       <c r="G20" s="3"/>
@@ -1098,7 +1132,9 @@
       <c r="A21" s="3"/>
       <c r="B21" s="2"/>
       <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
+      <c r="D21" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="E21" s="3"/>
       <c r="F21" s="2"/>
       <c r="G21" s="3"/>

</xml_diff>